<commit_message>
changes new analysis (volume and weight)
</commit_message>
<xml_diff>
--- a/analysis_VW/raw_data/TFE_volume_weigth.xlsx
+++ b/analysis_VW/raw_data/TFE_volume_weigth.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\PastHuman_StoneToolPerformance\analysis_VW\raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schunk\Documents\GitHub\PastHuman_StoneToolPerformance\analysis_VW\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CB29DA-2B4D-4AF7-B157-E5A514DE9224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD793FBF-B5F5-4DAB-9F8D-CC4E3BEFBD47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C4483967-44F0-491A-BF23-256605DBFF95}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4483967-44F0-491A-BF23-256605DBFF95}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="42">
   <si>
     <t>FLT8-1</t>
   </si>
@@ -147,16 +147,37 @@
   </si>
   <si>
     <t>lydite</t>
+  </si>
+  <si>
+    <t>cutting_45</t>
+  </si>
+  <si>
+    <t>cutting_35</t>
+  </si>
+  <si>
+    <t>carving_35</t>
+  </si>
+  <si>
+    <t>carving_45</t>
+  </si>
+  <si>
+    <t>motion_angle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -182,11 +203,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -202,7 +226,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -498,19 +522,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92985D24-EDBB-4D4D-B4CB-EC396D74E3CB}">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="1"/>
+    <col min="6" max="6" width="12.5546875" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -520,20 +546,23 @@
       <c r="C1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
       <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -543,20 +572,23 @@
       <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2">
-        <v>45</v>
-      </c>
-      <c r="F2">
+      <c r="D2" s="1">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2">
         <v>10350.700000000001</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>26.78</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -566,20 +598,23 @@
       <c r="C3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3">
-        <v>45</v>
-      </c>
-      <c r="F3">
+      <c r="D3" s="1">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3">
         <v>10401.4</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>26.85</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -589,20 +624,23 @@
       <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4">
-        <v>45</v>
-      </c>
-      <c r="F4">
+      <c r="D4" s="1">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4">
         <v>12569.3</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>32.270000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -612,20 +650,23 @@
       <c r="C5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5">
-        <v>35</v>
-      </c>
-      <c r="F5">
+      <c r="D5" s="1">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5">
         <v>10221.200000000001</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>26.46</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -635,20 +676,23 @@
       <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6">
-        <v>35</v>
-      </c>
-      <c r="F6">
+      <c r="D6" s="1">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6">
         <v>8530.4</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>22.01</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -658,20 +702,23 @@
       <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7">
-        <v>35</v>
-      </c>
-      <c r="F7">
+      <c r="D7" s="1">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7">
         <v>8007.6</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>20.83</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -681,20 +728,23 @@
       <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8">
-        <v>35</v>
-      </c>
-      <c r="F8">
+      <c r="D8" s="1">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8">
         <v>11276.6</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>29.25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -704,20 +754,23 @@
       <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9">
-        <v>35</v>
-      </c>
-      <c r="F9">
+      <c r="D9" s="1">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9">
         <v>13094</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>33.799999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -727,20 +780,23 @@
       <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10">
-        <v>35</v>
-      </c>
-      <c r="F10">
+      <c r="D10" s="1">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10">
         <v>9025.7000000000007</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>23.45</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -750,20 +806,23 @@
       <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="D11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11">
-        <v>45</v>
-      </c>
-      <c r="F11">
+      <c r="D11" s="1">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11">
         <v>9366.9</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>24.28</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -773,20 +832,23 @@
       <c r="C12" t="s">
         <v>28</v>
       </c>
-      <c r="D12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12">
-        <v>45</v>
-      </c>
-      <c r="F12">
+      <c r="D12" s="1">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12">
         <v>8774.2999999999993</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>22.83</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -796,20 +858,23 @@
       <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13">
-        <v>45</v>
-      </c>
-      <c r="F13">
+      <c r="D13" s="1">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13">
         <v>9288.6</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>23.97</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -819,20 +884,23 @@
       <c r="C14" t="s">
         <v>27</v>
       </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14">
-        <v>45</v>
-      </c>
-      <c r="F14">
+      <c r="D14" s="1">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14">
         <v>10303.9</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>26.77</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -842,20 +910,23 @@
       <c r="C15" t="s">
         <v>27</v>
       </c>
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15">
-        <v>45</v>
-      </c>
-      <c r="F15">
+      <c r="D15" s="1">
+        <v>45</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15">
         <v>10342.799999999999</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>26.84</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -865,20 +936,23 @@
       <c r="C16" t="s">
         <v>27</v>
       </c>
-      <c r="D16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16">
-        <v>45</v>
-      </c>
-      <c r="F16">
+      <c r="D16" s="1">
+        <v>45</v>
+      </c>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16">
         <v>12466.9</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>32.19</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -888,20 +962,23 @@
       <c r="C17" t="s">
         <v>27</v>
       </c>
-      <c r="D17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17">
-        <v>35</v>
-      </c>
-      <c r="F17">
+      <c r="D17" s="1">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17">
         <v>10217.299999999999</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>26.44</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -911,20 +988,23 @@
       <c r="C18" t="s">
         <v>27</v>
       </c>
-      <c r="D18" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18">
-        <v>35</v>
-      </c>
-      <c r="F18">
+      <c r="D18" s="1">
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18">
         <v>8443.7000000000007</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>21.99</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -934,20 +1014,23 @@
       <c r="C19" t="s">
         <v>27</v>
       </c>
-      <c r="D19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19">
-        <v>35</v>
-      </c>
-      <c r="F19">
+      <c r="D19" s="1">
+        <v>35</v>
+      </c>
+      <c r="E19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19">
         <v>7976.5</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>20.82</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -957,20 +1040,23 @@
       <c r="C20" t="s">
         <v>28</v>
       </c>
-      <c r="D20" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20">
-        <v>35</v>
-      </c>
-      <c r="F20">
+      <c r="D20" s="1">
+        <v>35</v>
+      </c>
+      <c r="E20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20">
         <v>11267.8</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>29.24</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -980,20 +1066,23 @@
       <c r="C21" t="s">
         <v>28</v>
       </c>
-      <c r="D21" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21">
-        <v>35</v>
-      </c>
-      <c r="F21">
+      <c r="D21" s="1">
+        <v>35</v>
+      </c>
+      <c r="E21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21">
         <v>13065.9</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>33.79</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1003,20 +1092,23 @@
       <c r="C22" t="s">
         <v>28</v>
       </c>
-      <c r="D22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22">
-        <v>35</v>
-      </c>
-      <c r="F22">
+      <c r="D22" s="1">
+        <v>35</v>
+      </c>
+      <c r="E22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22">
         <v>9005.2000000000007</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>23.44</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1026,20 +1118,23 @@
       <c r="C23" t="s">
         <v>28</v>
       </c>
-      <c r="D23" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23">
-        <v>45</v>
-      </c>
-      <c r="F23">
+      <c r="D23" s="1">
+        <v>45</v>
+      </c>
+      <c r="E23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23">
         <v>9216.2000000000007</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>23.69</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1049,20 +1144,23 @@
       <c r="C24" t="s">
         <v>28</v>
       </c>
-      <c r="D24" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24">
-        <v>45</v>
-      </c>
-      <c r="F24">
+      <c r="D24" s="1">
+        <v>45</v>
+      </c>
+      <c r="E24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24">
         <v>8771.6</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>22.82</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -1072,20 +1170,23 @@
       <c r="C25" t="s">
         <v>28</v>
       </c>
-      <c r="D25" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25">
-        <v>45</v>
-      </c>
-      <c r="F25">
+      <c r="D25" s="1">
+        <v>45</v>
+      </c>
+      <c r="E25" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25">
         <v>9224.6</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>23.96</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -1095,20 +1196,23 @@
       <c r="C26" t="s">
         <v>27</v>
       </c>
-      <c r="D26" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26">
-        <v>45</v>
-      </c>
-      <c r="F26">
+      <c r="D26" s="1">
+        <v>45</v>
+      </c>
+      <c r="E26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" t="s">
+        <v>37</v>
+      </c>
+      <c r="G26">
         <v>6077.2</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>15.85</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1118,20 +1222,23 @@
       <c r="C27" t="s">
         <v>27</v>
       </c>
-      <c r="D27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27">
-        <v>45</v>
-      </c>
-      <c r="F27">
+      <c r="D27" s="1">
+        <v>45</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27">
         <v>6353.4</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>16.63</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1141,20 +1248,23 @@
       <c r="C28" t="s">
         <v>27</v>
       </c>
-      <c r="D28" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28">
-        <v>45</v>
-      </c>
-      <c r="F28">
+      <c r="D28" s="1">
+        <v>45</v>
+      </c>
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G28">
         <v>7305</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>19.149999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -1164,20 +1274,23 @@
       <c r="C29" t="s">
         <v>27</v>
       </c>
-      <c r="D29" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29">
-        <v>35</v>
-      </c>
-      <c r="F29">
+      <c r="D29" s="1">
+        <v>35</v>
+      </c>
+      <c r="E29" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29">
         <v>8521.2999999999993</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>22.77</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1187,20 +1300,23 @@
       <c r="C30" t="s">
         <v>27</v>
       </c>
-      <c r="D30" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30">
-        <v>35</v>
-      </c>
-      <c r="F30">
+      <c r="D30" s="1">
+        <v>35</v>
+      </c>
+      <c r="E30" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30">
         <v>9169.2000000000007</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>24.02</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -1210,20 +1326,23 @@
       <c r="C31" t="s">
         <v>27</v>
       </c>
-      <c r="D31" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31">
-        <v>35</v>
-      </c>
-      <c r="F31">
+      <c r="D31" s="1">
+        <v>35</v>
+      </c>
+      <c r="E31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G31">
         <v>8457</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>22.1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -1233,20 +1352,23 @@
       <c r="C32" t="s">
         <v>28</v>
       </c>
-      <c r="D32" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32">
-        <v>45</v>
-      </c>
-      <c r="F32">
+      <c r="D32" s="1">
+        <v>45</v>
+      </c>
+      <c r="E32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G32">
         <v>9757.9</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>25.55</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -1256,20 +1378,23 @@
       <c r="C33" t="s">
         <v>28</v>
       </c>
-      <c r="D33" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33">
-        <v>45</v>
-      </c>
-      <c r="F33">
+      <c r="D33" s="1">
+        <v>45</v>
+      </c>
+      <c r="E33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33">
         <v>10808.3</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>28.39</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1279,20 +1404,23 @@
       <c r="C34" t="s">
         <v>28</v>
       </c>
-      <c r="D34" t="s">
-        <v>30</v>
-      </c>
-      <c r="E34">
-        <v>45</v>
-      </c>
-      <c r="F34">
+      <c r="D34" s="1">
+        <v>45</v>
+      </c>
+      <c r="E34" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G34">
         <v>9895.7000000000007</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>26.19</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -1302,20 +1430,23 @@
       <c r="C35" t="s">
         <v>28</v>
       </c>
-      <c r="D35" t="s">
-        <v>30</v>
-      </c>
-      <c r="E35">
-        <v>35</v>
-      </c>
-      <c r="F35">
+      <c r="D35" s="1">
+        <v>35</v>
+      </c>
+      <c r="E35" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35">
         <v>10027.1</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>26.46</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1325,20 +1456,23 @@
       <c r="C36" t="s">
         <v>28</v>
       </c>
-      <c r="D36" t="s">
-        <v>30</v>
-      </c>
-      <c r="E36">
-        <v>35</v>
-      </c>
-      <c r="F36">
+      <c r="D36" s="1">
+        <v>35</v>
+      </c>
+      <c r="E36" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36">
         <v>8792.1</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>23.14</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -1348,20 +1482,23 @@
       <c r="C37" t="s">
         <v>28</v>
       </c>
-      <c r="D37" t="s">
-        <v>30</v>
-      </c>
-      <c r="E37">
-        <v>35</v>
-      </c>
-      <c r="F37">
+      <c r="D37" s="1">
+        <v>35</v>
+      </c>
+      <c r="E37" t="s">
+        <v>30</v>
+      </c>
+      <c r="F37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G37">
         <v>8691.2999999999993</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>22.78</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -1371,20 +1508,23 @@
       <c r="C38" t="s">
         <v>27</v>
       </c>
-      <c r="D38" t="s">
-        <v>31</v>
-      </c>
-      <c r="E38">
-        <v>45</v>
-      </c>
-      <c r="F38">
+      <c r="D38" s="1">
+        <v>45</v>
+      </c>
+      <c r="E38" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38" t="s">
+        <v>37</v>
+      </c>
+      <c r="G38">
         <v>6066.3</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>15.84</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -1394,20 +1534,23 @@
       <c r="C39" t="s">
         <v>27</v>
       </c>
-      <c r="D39" t="s">
-        <v>31</v>
-      </c>
-      <c r="E39">
-        <v>45</v>
-      </c>
-      <c r="F39">
+      <c r="D39" s="1">
+        <v>45</v>
+      </c>
+      <c r="E39" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" t="s">
+        <v>37</v>
+      </c>
+      <c r="G39">
         <v>6351.7</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>16.63</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -1417,20 +1560,23 @@
       <c r="C40" t="s">
         <v>27</v>
       </c>
-      <c r="D40" t="s">
-        <v>31</v>
-      </c>
-      <c r="E40">
-        <v>45</v>
-      </c>
-      <c r="F40">
+      <c r="D40" s="1">
+        <v>45</v>
+      </c>
+      <c r="E40" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" t="s">
+        <v>37</v>
+      </c>
+      <c r="G40">
         <v>7279</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>19.13</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>15</v>
       </c>
@@ -1440,20 +1586,23 @@
       <c r="C41" t="s">
         <v>27</v>
       </c>
-      <c r="D41" t="s">
-        <v>31</v>
-      </c>
-      <c r="E41">
-        <v>35</v>
-      </c>
-      <c r="F41">
+      <c r="D41" s="1">
+        <v>35</v>
+      </c>
+      <c r="E41" t="s">
+        <v>31</v>
+      </c>
+      <c r="F41" t="s">
+        <v>38</v>
+      </c>
+      <c r="G41">
         <v>8315.5</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>21.85</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -1463,20 +1612,23 @@
       <c r="C42" t="s">
         <v>27</v>
       </c>
-      <c r="D42" t="s">
-        <v>31</v>
-      </c>
-      <c r="E42">
-        <v>35</v>
-      </c>
-      <c r="F42">
+      <c r="D42" s="1">
+        <v>35</v>
+      </c>
+      <c r="E42" t="s">
+        <v>31</v>
+      </c>
+      <c r="F42" t="s">
+        <v>38</v>
+      </c>
+      <c r="G42">
         <v>9161.2000000000007</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>23.99</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -1486,20 +1638,23 @@
       <c r="C43" t="s">
         <v>27</v>
       </c>
-      <c r="D43" t="s">
-        <v>31</v>
-      </c>
-      <c r="E43">
-        <v>35</v>
-      </c>
-      <c r="F43">
+      <c r="D43" s="1">
+        <v>35</v>
+      </c>
+      <c r="E43" t="s">
+        <v>31</v>
+      </c>
+      <c r="F43" t="s">
+        <v>38</v>
+      </c>
+      <c r="G43">
         <v>8396.7000000000007</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>22.07</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>18</v>
       </c>
@@ -1509,20 +1664,23 @@
       <c r="C44" t="s">
         <v>28</v>
       </c>
-      <c r="D44" t="s">
-        <v>31</v>
-      </c>
-      <c r="E44">
-        <v>45</v>
-      </c>
-      <c r="F44">
+      <c r="D44" s="1">
+        <v>45</v>
+      </c>
+      <c r="E44" t="s">
+        <v>31</v>
+      </c>
+      <c r="F44" t="s">
+        <v>40</v>
+      </c>
+      <c r="G44">
         <v>9728.1</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>25.53</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -1532,20 +1690,23 @@
       <c r="C45" t="s">
         <v>28</v>
       </c>
-      <c r="D45" t="s">
-        <v>31</v>
-      </c>
-      <c r="E45">
-        <v>45</v>
-      </c>
-      <c r="F45">
+      <c r="D45" s="1">
+        <v>45</v>
+      </c>
+      <c r="E45" t="s">
+        <v>31</v>
+      </c>
+      <c r="F45" t="s">
+        <v>40</v>
+      </c>
+      <c r="G45">
         <v>10784.9</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>28.35</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>20</v>
       </c>
@@ -1555,20 +1716,23 @@
       <c r="C46" t="s">
         <v>28</v>
       </c>
-      <c r="D46" t="s">
-        <v>31</v>
-      </c>
-      <c r="E46">
-        <v>45</v>
-      </c>
-      <c r="F46">
+      <c r="D46" s="1">
+        <v>45</v>
+      </c>
+      <c r="E46" t="s">
+        <v>31</v>
+      </c>
+      <c r="F46" t="s">
+        <v>40</v>
+      </c>
+      <c r="G46">
         <v>9873.7000000000007</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <v>26.18</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>21</v>
       </c>
@@ -1578,20 +1742,23 @@
       <c r="C47" t="s">
         <v>28</v>
       </c>
-      <c r="D47" t="s">
-        <v>31</v>
-      </c>
-      <c r="E47">
-        <v>35</v>
-      </c>
-      <c r="F47">
+      <c r="D47" s="1">
+        <v>35</v>
+      </c>
+      <c r="E47" t="s">
+        <v>31</v>
+      </c>
+      <c r="F47" t="s">
+        <v>39</v>
+      </c>
+      <c r="G47">
         <v>10021.4</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>26.45</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>22</v>
       </c>
@@ -1601,20 +1768,23 @@
       <c r="C48" t="s">
         <v>28</v>
       </c>
-      <c r="D48" t="s">
-        <v>31</v>
-      </c>
-      <c r="E48">
-        <v>35</v>
-      </c>
-      <c r="F48">
+      <c r="D48" s="1">
+        <v>35</v>
+      </c>
+      <c r="E48" t="s">
+        <v>31</v>
+      </c>
+      <c r="F48" t="s">
+        <v>39</v>
+      </c>
+      <c r="G48">
         <v>8769.6</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>23.14</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>23</v>
       </c>
@@ -1624,20 +1794,24 @@
       <c r="C49" t="s">
         <v>28</v>
       </c>
-      <c r="D49" t="s">
-        <v>31</v>
-      </c>
-      <c r="E49">
-        <v>35</v>
-      </c>
-      <c r="F49">
+      <c r="D49" s="1">
+        <v>35</v>
+      </c>
+      <c r="E49" t="s">
+        <v>31</v>
+      </c>
+      <c r="F49" t="s">
+        <v>39</v>
+      </c>
+      <c r="G49">
         <v>8668.1</v>
       </c>
-      <c r="G49">
+      <c r="H49">
         <v>22.78</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>